<commit_message>
Update: tracability matrix -1
</commit_message>
<xml_diff>
--- a/Documents/old-docs/TraceabilityMatrix(DM-UC).xlsx
+++ b/Documents/old-docs/TraceabilityMatrix(DM-UC).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\han\Downloads\3학년 1학기\소프트웨어 공학\Warehouse-Management-System\Documents\Domain model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\han\Downloads\3학년 1학기\소프트웨어 공학\Warehouse-Management-System\Documents\old-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C427487F-995A-4932-8227-A5DB9E1E9990}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C54E04E-D00A-41E8-A969-58A729B12FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4515" yWindow="645" windowWidth="32220" windowHeight="14490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8355" yWindow="585" windowWidth="22095" windowHeight="14490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="77">
   <si>
     <t>Warehouse</t>
   </si>
@@ -81,9 +81,6 @@
     <t>UserModuleConnection</t>
   </si>
   <si>
-    <t>ViewPage</t>
-  </si>
-  <si>
     <t>PageInfo</t>
   </si>
   <si>
@@ -97,12 +94,6 @@
   </si>
   <si>
     <t>Notifier</t>
-  </si>
-  <si>
-    <t>Agree</t>
-  </si>
-  <si>
-    <t>Refuse</t>
   </si>
   <si>
     <t>Accounts</t>
@@ -251,6 +242,22 @@
   </si>
   <si>
     <t>UC-09</t>
+  </si>
+  <si>
+    <t>PageMaker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompareAccount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompareResult</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -737,8 +744,8 @@
   </sheetPr>
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AB18" sqref="AB18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -751,76 +758,76 @@
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="X1" s="4"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3">
         <v>17</v>
@@ -895,22 +902,22 @@
         <v>14</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -935,19 +942,13 @@
         <v>15</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -970,18 +971,20 @@
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="D5" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="7"/>
+        <v>59</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -991,7 +994,7 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
@@ -1007,10 +1010,10 @@
         <v>17</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -1039,23 +1042,19 @@
         <v>18</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>62</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>62</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -1065,7 +1064,7 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
@@ -1078,26 +1077,28 @@
     </row>
     <row r="8" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7" t="s">
-        <v>62</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="7"/>
+        <v>59</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
@@ -1105,45 +1106,47 @@
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="V8" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="W8" s="7"/>
       <c r="X8" s="5"/>
     </row>
     <row r="9" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
-        <v>62</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="7"/>
+        <v>59</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
@@ -1151,29 +1154,29 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="T9" s="7"/>
       <c r="U9" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="V9" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="W9" s="7"/>
       <c r="X9" s="5"/>
     </row>
     <row r="10" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -1198,12 +1201,12 @@
     </row>
     <row r="11" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1228,13 +1231,13 @@
     </row>
     <row r="12" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="8"/>
@@ -1244,13 +1247,13 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
@@ -1262,16 +1265,14 @@
     </row>
     <row r="13" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>62</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -1294,7 +1295,7 @@
     </row>
     <row r="14" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1302,12 +1303,12 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
+      <c r="I14" s="7"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
+      <c r="K14" s="8"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
@@ -1324,23 +1325,27 @@
     </row>
     <row r="15" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="J15" s="7"/>
-      <c r="K15" s="8"/>
+      <c r="K15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
+      <c r="N15" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
@@ -1354,22 +1359,20 @@
     </row>
     <row r="16" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>62</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="8"/>
+      <c r="K16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
@@ -1386,27 +1389,23 @@
     </row>
     <row r="17" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="G17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
-      <c r="N17" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
@@ -1427,58 +1426,58 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M18" s="7"/>
       <c r="N18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="U18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="W18" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="X18" s="5"/>
     </row>
     <row r="19" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1487,22 +1486,22 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
@@ -1518,7 +1517,7 @@
     </row>
     <row r="20" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1527,7 +1526,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
@@ -1548,7 +1547,7 @@
     </row>
     <row r="21" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1557,20 +1556,20 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
       <c r="N21" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
@@ -1584,7 +1583,7 @@
     </row>
     <row r="22" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1594,7 +1593,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
@@ -1614,7 +1613,7 @@
     </row>
     <row r="23" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1625,7 +1624,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
@@ -1644,7 +1643,7 @@
     </row>
     <row r="24" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1655,7 +1654,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
@@ -1674,7 +1673,7 @@
     </row>
     <row r="25" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1685,7 +1684,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
@@ -1704,7 +1703,7 @@
     </row>
     <row r="26" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1716,7 +1715,7 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
@@ -1734,7 +1733,7 @@
     </row>
     <row r="27" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1746,7 +1745,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
@@ -1764,7 +1763,7 @@
     </row>
     <row r="28" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1776,7 +1775,7 @@
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
@@ -1794,7 +1793,7 @@
     </row>
     <row r="29" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1806,7 +1805,7 @@
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
@@ -1824,7 +1823,7 @@
     </row>
     <row r="30" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1836,7 +1835,7 @@
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
@@ -1854,7 +1853,7 @@
     </row>
     <row r="31" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1869,22 +1868,22 @@
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
       <c r="N31" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O31" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Q31" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="R31" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="S31" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>
@@ -1894,7 +1893,7 @@
     </row>
     <row r="32" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1907,7 +1906,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
       <c r="L32" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
@@ -1924,7 +1923,7 @@
     </row>
     <row r="33" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1937,7 +1936,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
       <c r="L33" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
@@ -1954,7 +1953,7 @@
     </row>
     <row r="34" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1967,7 +1966,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
       <c r="L34" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
@@ -1984,7 +1983,7 @@
     </row>
     <row r="35" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1998,7 +1997,7 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
@@ -2014,7 +2013,7 @@
     </row>
     <row r="36" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -2028,15 +2027,15 @@
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
       <c r="P36" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Q36" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="R36" s="7"/>
       <c r="S36" s="7"/>
@@ -2048,7 +2047,7 @@
     </row>
     <row r="37" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -2063,7 +2062,7 @@
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
       <c r="N37" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O37" s="7"/>
       <c r="P37" s="7"/>
@@ -2078,7 +2077,7 @@
     </row>
     <row r="38" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -2094,11 +2093,11 @@
       <c r="M38" s="7"/>
       <c r="N38" s="7"/>
       <c r="O38" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P38" s="7"/>
       <c r="Q38" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="R38" s="7"/>
       <c r="S38" s="7"/>
@@ -2110,7 +2109,7 @@
     </row>
     <row r="39" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -2123,7 +2122,7 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
       <c r="L39" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M39" s="7"/>
       <c r="N39" s="7"/>
@@ -2140,7 +2139,7 @@
     </row>
     <row r="40" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -2159,7 +2158,7 @@
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
       <c r="R40" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="S40" s="7"/>
       <c r="T40" s="7"/>
@@ -2190,7 +2189,7 @@
       <c r="Q41" s="7"/>
       <c r="R41" s="7"/>
       <c r="S41" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="T41" s="7"/>
       <c r="U41" s="7"/>
@@ -2200,7 +2199,7 @@
     </row>
     <row r="42" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -2221,16 +2220,16 @@
       <c r="R42" s="7"/>
       <c r="S42" s="7"/>
       <c r="T42" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="U42" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="V42" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="W42" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="X42" s="5"/>
     </row>
@@ -2257,7 +2256,7 @@
       <c r="R43" s="7"/>
       <c r="S43" s="7"/>
       <c r="T43" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="U43" s="7"/>
       <c r="V43" s="7"/>
@@ -2287,7 +2286,7 @@
       <c r="R44" s="7"/>
       <c r="S44" s="7"/>
       <c r="T44" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="U44" s="7"/>
       <c r="V44" s="7"/>
@@ -2318,7 +2317,7 @@
       <c r="S45" s="7"/>
       <c r="T45" s="7"/>
       <c r="U45" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="V45" s="7"/>
       <c r="W45" s="7"/>
@@ -2348,7 +2347,7 @@
       <c r="S46" s="7"/>
       <c r="T46" s="7"/>
       <c r="U46" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="V46" s="7"/>
       <c r="W46" s="7"/>
@@ -2378,7 +2377,7 @@
       <c r="S47" s="7"/>
       <c r="T47" s="7"/>
       <c r="U47" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="V47" s="7"/>
       <c r="W47" s="7"/>
@@ -2408,7 +2407,7 @@
       <c r="S48" s="7"/>
       <c r="T48" s="7"/>
       <c r="U48" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="V48" s="7"/>
       <c r="W48" s="7"/>
@@ -2439,7 +2438,7 @@
       <c r="T49" s="7"/>
       <c r="U49" s="7"/>
       <c r="V49" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="W49" s="7"/>
       <c r="X49" s="5"/>
@@ -2469,7 +2468,7 @@
       <c r="T50" s="7"/>
       <c r="U50" s="7"/>
       <c r="V50" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="W50" s="7"/>
       <c r="X50" s="5"/>
@@ -2499,7 +2498,7 @@
       <c r="T51" s="7"/>
       <c r="U51" s="7"/>
       <c r="V51" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="W51" s="7"/>
       <c r="X51" s="5"/>
@@ -2530,7 +2529,7 @@
       <c r="U52" s="7"/>
       <c r="V52" s="7"/>
       <c r="W52" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="X52" s="5"/>
     </row>
@@ -2560,7 +2559,7 @@
       <c r="U53" s="7"/>
       <c r="V53" s="7"/>
       <c r="W53" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="X53" s="5"/>
     </row>
@@ -2590,7 +2589,7 @@
       <c r="U54" s="7"/>
       <c r="V54" s="7"/>
       <c r="W54" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="X54" s="5"/>
     </row>

</xml_diff>